<commit_message>
renew hw 562 565
</commit_message>
<xml_diff>
--- a/docs/stat565/Exercise3_22.xlsx
+++ b/docs/stat565/Exercise3_22.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadeej2\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="5190"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
   <si>
     <t>Type</t>
   </si>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,6 +92,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -134,7 +142,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -169,7 +177,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,9 +386,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -502,6 +512,14 @@
       </c>
       <c r="B15">
         <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>